<commit_message>
Resolve "write test for CubeController"
</commit_message>
<xml_diff>
--- a/time-records/Fritz Verena_c7031304.xlsx
+++ b/time-records/Fritz Verena_c7031304.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bolia\Documents\erweiterungsstudium\swe\PS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473B2722-C607-4F0A-9F4E-42DFC652B3B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCAB026-C7D2-4BB7-AF54-68C4243754FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="33750" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>Datum</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>Test CubeStatusController</t>
+  </si>
+  <si>
+    <t>CubeController Test</t>
+  </si>
+  <si>
+    <t>Runde beenden durch Timer</t>
   </si>
 </sst>
 </file>
@@ -659,7 +665,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomRight" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1447,14 +1453,32 @@
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="5"/>
-      <c r="B57" s="6"/>
-      <c r="D57" s="8"/>
+      <c r="A57" s="5">
+        <v>44322</v>
+      </c>
+      <c r="B57" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6"/>
-      <c r="D58" s="8"/>
+      <c r="A58" s="5">
+        <v>44323</v>
+      </c>
+      <c r="B58" s="6">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="5"/>

</xml_diff>